<commit_message>
ums-commons/改进: 添加 TableId 的 IdType 类型.
</commit_message>
<xml_diff>
--- a/arch-ums/uni-life-ums.xlsx
+++ b/arch-ums/uni-life-ums.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces-Idea\proc\arch-module\arch-ums\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE5FB9C1-6021-42A1-A99D-468D4818ADEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA1CF1E-3223-43CC-A257-B41D4C265D97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="4296" windowWidth="23040" windowHeight="12312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="867">
   <si>
     <t>表名/Table</t>
   </si>
@@ -2454,10 +2454,6 @@
   </si>
   <si>
     <t>来源，推广统计用</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名ID</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -3161,8 +3157,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3170,14 +3166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4459,7 +4455,7 @@
         <v>745</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>11</v>
@@ -4485,7 +4481,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
       <c r="B3" s="26" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>17</v>
@@ -4625,7 +4621,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="26" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>17</v>
@@ -4750,7 +4746,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
       <c r="B17" s="43" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>709</v>
@@ -4764,7 +4760,7 @@
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="39" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -4800,7 +4796,7 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="50"/>
       <c r="B20" s="39" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C20" s="40" t="s">
         <v>708</v>
@@ -4814,7 +4810,7 @@
       <c r="H20" s="42"/>
       <c r="I20" s="42"/>
       <c r="J20" s="39" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -4951,7 +4947,7 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="50"/>
       <c r="B29" s="26" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C29" s="23" t="s">
         <v>17</v>
@@ -5024,7 +5020,7 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="26" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>17</v>
@@ -7672,8 +7668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7723,11 +7719,11 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
-        <v>857</v>
+      <c r="A2" s="52" t="s">
+        <v>856</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>17</v>
@@ -7741,13 +7737,13 @@
       <c r="H2" s="31"/>
       <c r="I2" s="30"/>
       <c r="J2" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="29" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>709</v>
@@ -7765,7 +7761,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="33" t="s">
         <v>752</v>
       </c>
@@ -7781,13 +7777,13 @@
       <c r="H4" s="36"/>
       <c r="I4" s="36"/>
       <c r="J4" s="49" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="29" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>709</v>
@@ -7915,13 +7911,13 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="54"/>
       <c r="B11" s="37" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>11</v>
@@ -7935,7 +7931,7 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="35" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -8458,13 +8454,13 @@
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="27" t="s">
-        <v>770</v>
+        <v>720</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="54"/>
       <c r="B35" s="29" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>17</v>
@@ -8490,7 +8486,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="54"/>
       <c r="B36" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C36" s="44" t="s">
         <v>709</v>
@@ -8504,13 +8500,13 @@
       <c r="H36" s="48"/>
       <c r="I36" s="48"/>
       <c r="J36" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="54"/>
       <c r="B37" s="47" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C37" s="44" t="s">
         <v>709</v>
@@ -8524,7 +8520,7 @@
       <c r="H37" s="48"/>
       <c r="I37" s="48"/>
       <c r="J37" s="46" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -8536,7 +8532,7 @@
         <v>17</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>13</v>
@@ -8576,7 +8572,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="55" t="s">
         <v>727</v>
       </c>
       <c r="B40" s="21" t="s">
@@ -8598,7 +8594,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="21" t="s">
         <v>125</v>
       </c>
@@ -8614,11 +8610,11 @@
       <c r="H41" s="24"/>
       <c r="I41" s="24"/>
       <c r="J41" s="27" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="57"/>
+      <c r="A42" s="56"/>
       <c r="B42" s="21" t="s">
         <v>126</v>
       </c>
@@ -8634,11 +8630,11 @@
       <c r="H42" s="24"/>
       <c r="I42" s="24"/>
       <c r="J42" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
+      <c r="A43" s="56"/>
       <c r="B43" s="21" t="s">
         <v>127</v>
       </c>
@@ -8654,11 +8650,11 @@
       <c r="H43" s="24"/>
       <c r="I43" s="24"/>
       <c r="J43" s="27" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
+      <c r="A44" s="56"/>
       <c r="B44" s="21" t="s">
         <v>128</v>
       </c>
@@ -8674,11 +8670,11 @@
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
       <c r="J44" s="27" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="21" t="s">
         <v>129</v>
       </c>
@@ -8694,11 +8690,11 @@
       <c r="H45" s="24"/>
       <c r="I45" s="24"/>
       <c r="J45" s="27" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="21" t="s">
         <v>130</v>
       </c>
@@ -8714,11 +8710,11 @@
       <c r="H46" s="24"/>
       <c r="I46" s="24"/>
       <c r="J46" s="27" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="21" t="s">
         <v>131</v>
       </c>
@@ -8734,11 +8730,11 @@
       <c r="H47" s="24"/>
       <c r="I47" s="24"/>
       <c r="J47" s="27" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="21" t="s">
         <v>132</v>
       </c>
@@ -8754,11 +8750,11 @@
       <c r="H48" s="24"/>
       <c r="I48" s="24"/>
       <c r="J48" s="27" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="21" t="s">
         <v>133</v>
       </c>
@@ -8774,7 +8770,7 @@
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
       <c r="J49" s="27" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -8802,13 +8798,13 @@
       </c>
       <c r="I50" s="23"/>
       <c r="J50" s="27" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="53"/>
       <c r="B51" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C51" s="44" t="s">
         <v>709</v>
@@ -8822,7 +8818,7 @@
       <c r="H51" s="48"/>
       <c r="I51" s="48"/>
       <c r="J51" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -8848,7 +8844,7 @@
       </c>
       <c r="I52" s="23"/>
       <c r="J52" s="27" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -8870,15 +8866,15 @@
       <c r="H53" s="10"/>
       <c r="I53" s="23"/>
       <c r="J53" s="27" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="53" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>11</v>
@@ -8892,13 +8888,13 @@
       <c r="H54" s="10"/>
       <c r="I54" s="23"/>
       <c r="J54" s="27" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="54"/>
       <c r="B55" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C55" s="44" t="s">
         <v>709</v>
@@ -8912,7 +8908,7 @@
       <c r="H55" s="48"/>
       <c r="I55" s="48"/>
       <c r="J55" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -8932,7 +8928,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="23"/>
       <c r="J56" s="27" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -8952,12 +8948,12 @@
       <c r="H57" s="10"/>
       <c r="I57" s="23"/>
       <c r="J57" s="27" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="53" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>139</v>
@@ -8974,13 +8970,13 @@
       <c r="H58" s="10"/>
       <c r="I58" s="23"/>
       <c r="J58" s="27" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="54"/>
       <c r="B59" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C59" s="44" t="s">
         <v>709</v>
@@ -8994,7 +8990,7 @@
       <c r="H59" s="48"/>
       <c r="I59" s="48"/>
       <c r="J59" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -9014,7 +9010,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="23"/>
       <c r="J60" s="27" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -9034,13 +9030,13 @@
       <c r="H61" s="10"/>
       <c r="I61" s="23"/>
       <c r="J61" s="27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="54"/>
       <c r="B62" s="21" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>17</v>
@@ -9054,7 +9050,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="23"/>
       <c r="J62" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -9074,7 +9070,7 @@
       <c r="H63" s="10"/>
       <c r="I63" s="23"/>
       <c r="J63" s="27" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -9094,7 +9090,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="23"/>
       <c r="J64" s="27" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -9114,7 +9110,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="23"/>
       <c r="J65" s="27" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -9134,7 +9130,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="23"/>
       <c r="J66" s="27" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -9154,7 +9150,7 @@
       <c r="H67" s="10"/>
       <c r="I67" s="23"/>
       <c r="J67" s="27" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -9174,12 +9170,12 @@
       <c r="H68" s="10"/>
       <c r="I68" s="23"/>
       <c r="J68" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="53" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B69" s="21" t="s">
         <v>124</v>
@@ -9196,13 +9192,13 @@
       <c r="H69" s="10"/>
       <c r="I69" s="23"/>
       <c r="J69" s="27" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="54"/>
       <c r="B70" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C70" s="44" t="s">
         <v>709</v>
@@ -9216,7 +9212,7 @@
       <c r="H70" s="48"/>
       <c r="I70" s="48"/>
       <c r="J70" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -9236,7 +9232,7 @@
       <c r="H71" s="24"/>
       <c r="I71" s="24"/>
       <c r="J71" s="27" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -9256,7 +9252,7 @@
       <c r="H72" s="24"/>
       <c r="I72" s="24"/>
       <c r="J72" s="27" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -9276,7 +9272,7 @@
       <c r="H73" s="24"/>
       <c r="I73" s="24"/>
       <c r="J73" s="27" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -9296,7 +9292,7 @@
       <c r="H74" s="24"/>
       <c r="I74" s="24"/>
       <c r="J74" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -9316,7 +9312,7 @@
       <c r="H75" s="24"/>
       <c r="I75" s="24"/>
       <c r="J75" s="27" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -9336,7 +9332,7 @@
       <c r="H76" s="24"/>
       <c r="I76" s="24"/>
       <c r="J76" s="27" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -9356,15 +9352,15 @@
       <c r="H77" s="24"/>
       <c r="I77" s="24"/>
       <c r="J77" s="27" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="53" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B78" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C78" s="44" t="s">
         <v>709</v>
@@ -9378,7 +9374,7 @@
       <c r="H78" s="48"/>
       <c r="I78" s="48"/>
       <c r="J78" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -9418,7 +9414,7 @@
       <c r="H80" s="24"/>
       <c r="I80" s="24"/>
       <c r="J80" s="27" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -9438,7 +9434,7 @@
       <c r="H81" s="24"/>
       <c r="I81" s="24"/>
       <c r="J81" s="27" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -9458,13 +9454,13 @@
       <c r="H82" s="24"/>
       <c r="I82" s="24"/>
       <c r="J82" s="27" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="54"/>
       <c r="B83" s="29" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C83" s="22" t="s">
         <v>17</v>
@@ -9498,12 +9494,12 @@
       <c r="H84" s="24"/>
       <c r="I84" s="24"/>
       <c r="J84" s="27" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="53" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B85" s="21" t="s">
         <v>159</v>
@@ -9520,13 +9516,13 @@
       <c r="H85" s="24"/>
       <c r="I85" s="24"/>
       <c r="J85" s="27" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="54"/>
       <c r="B86" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C86" s="44" t="s">
         <v>709</v>
@@ -9540,7 +9536,7 @@
       <c r="H86" s="48"/>
       <c r="I86" s="48"/>
       <c r="J86" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -9560,7 +9556,7 @@
       <c r="H87" s="24"/>
       <c r="I87" s="24"/>
       <c r="J87" s="27" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -9580,7 +9576,7 @@
       <c r="H88" s="24"/>
       <c r="I88" s="24"/>
       <c r="J88" s="27" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -9600,7 +9596,7 @@
       <c r="H89" s="24"/>
       <c r="I89" s="24"/>
       <c r="J89" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -9620,12 +9616,12 @@
       <c r="H90" s="24"/>
       <c r="I90" s="24"/>
       <c r="J90" s="27" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="53" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B91" s="21" t="s">
         <v>162</v>
@@ -9642,13 +9638,13 @@
       <c r="H91" s="24"/>
       <c r="I91" s="24"/>
       <c r="J91" s="27" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="54"/>
       <c r="B92" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C92" s="44" t="s">
         <v>709</v>
@@ -9662,7 +9658,7 @@
       <c r="H92" s="48"/>
       <c r="I92" s="48"/>
       <c r="J92" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -9682,7 +9678,7 @@
       <c r="H93" s="24"/>
       <c r="I93" s="24"/>
       <c r="J93" s="27" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -9702,7 +9698,7 @@
       <c r="H94" s="24"/>
       <c r="I94" s="24"/>
       <c r="J94" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -9722,7 +9718,7 @@
       <c r="H95" s="24"/>
       <c r="I95" s="24"/>
       <c r="J95" s="27" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -9742,15 +9738,15 @@
       <c r="H96" s="24"/>
       <c r="I96" s="24"/>
       <c r="J96" s="27" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="53" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B97" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C97" s="44" t="s">
         <v>709</v>
@@ -9764,7 +9760,7 @@
       <c r="H97" s="48"/>
       <c r="I97" s="48"/>
       <c r="J97" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -9784,7 +9780,7 @@
       <c r="H98" s="24"/>
       <c r="I98" s="24"/>
       <c r="J98" s="27" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -9804,15 +9800,15 @@
       <c r="H99" s="24"/>
       <c r="I99" s="24"/>
       <c r="J99" s="27" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="53" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B100" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C100" s="44" t="s">
         <v>709</v>
@@ -9826,7 +9822,7 @@
       <c r="H100" s="48"/>
       <c r="I100" s="48"/>
       <c r="J100" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -9846,7 +9842,7 @@
       <c r="H101" s="24"/>
       <c r="I101" s="24"/>
       <c r="J101" s="27" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -9866,15 +9862,15 @@
       <c r="H102" s="24"/>
       <c r="I102" s="24"/>
       <c r="J102" s="27" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="53" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B103" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C103" s="44" t="s">
         <v>709</v>
@@ -9888,7 +9884,7 @@
       <c r="H103" s="48"/>
       <c r="I103" s="48"/>
       <c r="J103" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -9908,7 +9904,7 @@
       <c r="H104" s="24"/>
       <c r="I104" s="24"/>
       <c r="J104" s="27" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -9928,15 +9924,15 @@
       <c r="H105" s="24"/>
       <c r="I105" s="24"/>
       <c r="J105" s="27" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="53" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B106" s="47" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C106" s="44" t="s">
         <v>709</v>
@@ -9950,7 +9946,7 @@
       <c r="H106" s="48"/>
       <c r="I106" s="48"/>
       <c r="J106" s="46" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -9970,7 +9966,7 @@
       <c r="H107" s="24"/>
       <c r="I107" s="24"/>
       <c r="J107" s="27" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -9990,11 +9986,11 @@
       <c r="H108" s="24"/>
       <c r="I108" s="24"/>
       <c r="J108" s="27" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="52" t="s">
+      <c r="A109" s="57" t="s">
         <v>172</v>
       </c>
       <c r="B109" s="21" t="s">
@@ -10012,13 +10008,13 @@
       <c r="H109" s="24"/>
       <c r="I109" s="24"/>
       <c r="J109" s="27" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="52"/>
+      <c r="A110" s="57"/>
       <c r="B110" s="29" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C110" s="22" t="s">
         <v>17</v>
@@ -10032,11 +10028,11 @@
       <c r="H110" s="24"/>
       <c r="I110" s="24"/>
       <c r="J110" s="27" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="52"/>
+      <c r="A111" s="57"/>
       <c r="B111" s="21" t="s">
         <v>174</v>
       </c>
@@ -10052,11 +10048,11 @@
       <c r="H111" s="24"/>
       <c r="I111" s="24"/>
       <c r="J111" s="27" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="52"/>
+      <c r="A112" s="57"/>
       <c r="B112" s="21" t="s">
         <v>175</v>
       </c>
@@ -10072,11 +10068,11 @@
       <c r="H112" s="24"/>
       <c r="I112" s="24"/>
       <c r="J112" s="27" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="52" t="s">
+      <c r="A113" s="57" t="s">
         <v>176</v>
       </c>
       <c r="B113" s="21" t="s">
@@ -10094,11 +10090,11 @@
       <c r="H113" s="24"/>
       <c r="I113" s="24"/>
       <c r="J113" s="27" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="52"/>
+      <c r="A114" s="57"/>
       <c r="B114" s="21" t="s">
         <v>177</v>
       </c>
@@ -10114,11 +10110,11 @@
       <c r="H114" s="24"/>
       <c r="I114" s="24"/>
       <c r="J114" s="27" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="52"/>
+      <c r="A115" s="57"/>
       <c r="B115" s="21" t="s">
         <v>178</v>
       </c>
@@ -10134,11 +10130,11 @@
       <c r="H115" s="24"/>
       <c r="I115" s="24"/>
       <c r="J115" s="27" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="52"/>
+      <c r="A116" s="57"/>
       <c r="B116" s="21" t="s">
         <v>179</v>
       </c>
@@ -10154,11 +10150,11 @@
       <c r="H116" s="24"/>
       <c r="I116" s="24"/>
       <c r="J116" s="27" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="52" t="s">
+      <c r="A117" s="57" t="s">
         <v>180</v>
       </c>
       <c r="B117" s="21" t="s">
@@ -10176,11 +10172,11 @@
       <c r="H117" s="24"/>
       <c r="I117" s="24"/>
       <c r="J117" s="27" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="52"/>
+      <c r="A118" s="57"/>
       <c r="B118" s="21" t="s">
         <v>181</v>
       </c>
@@ -10196,11 +10192,11 @@
       <c r="H118" s="24"/>
       <c r="I118" s="24"/>
       <c r="J118" s="27" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="52"/>
+      <c r="A119" s="57"/>
       <c r="B119" s="21" t="s">
         <v>182</v>
       </c>
@@ -10214,11 +10210,11 @@
       <c r="H119" s="24"/>
       <c r="I119" s="24"/>
       <c r="J119" s="27" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="52"/>
+      <c r="A120" s="57"/>
       <c r="B120" s="21" t="s">
         <v>183</v>
       </c>
@@ -10232,12 +10228,12 @@
       <c r="H120" s="24"/>
       <c r="I120" s="24"/>
       <c r="J120" s="27" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="52" t="s">
-        <v>837</v>
+      <c r="A121" s="57" t="s">
+        <v>836</v>
       </c>
       <c r="B121" s="21" t="s">
         <v>107</v>
@@ -10254,13 +10250,13 @@
       <c r="H121" s="24"/>
       <c r="I121" s="24"/>
       <c r="J121" s="27" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="52"/>
+      <c r="A122" s="57"/>
       <c r="B122" s="29" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C122" s="22" t="s">
         <v>17</v>
@@ -10274,11 +10270,11 @@
       <c r="H122" s="24"/>
       <c r="I122" s="24"/>
       <c r="J122" s="27" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="52"/>
+      <c r="A123" s="57"/>
       <c r="B123" s="21" t="s">
         <v>184</v>
       </c>
@@ -10292,11 +10288,11 @@
       <c r="H123" s="24"/>
       <c r="I123" s="24"/>
       <c r="J123" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="52"/>
+      <c r="A124" s="57"/>
       <c r="B124" s="21" t="s">
         <v>185</v>
       </c>
@@ -10312,7 +10308,7 @@
       <c r="H124" s="24"/>
       <c r="I124" s="24"/>
       <c r="J124" s="27" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -10339,6 +10335,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A109:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A68"/>
+    <mergeCell ref="A78:A84"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A29"/>
     <mergeCell ref="A69:A77"/>
@@ -10348,17 +10355,6 @@
     <mergeCell ref="A40:A49"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A68"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A106:A108"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1">

</xml_diff>

<commit_message>
ums/新增: Relationship 新增 pseq 父节点顺序字段.
</commit_message>
<xml_diff>
--- a/arch-ums/uni-life-ums.xlsx
+++ b/arch-ums/uni-life-ums.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces-Idea\proc\arch-module\arch-ums\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595FC89-873E-41F7-B2A4-3E6A47BD3431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2598471-B5F1-40CB-B995-074CD61EBA2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5292" yWindow="2304" windowWidth="23040" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5292" yWindow="2304" windowWidth="23040" windowHeight="12312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="903">
   <si>
     <t>表名/Table</t>
   </si>
@@ -3101,6 +3101,17 @@
   </si>
   <si>
     <t>dt</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>pseq</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>父节点顺序</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -3381,8 +3392,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3390,14 +3401,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3405,12 +3410,88 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="75">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4044,41 +4125,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4318,41 +4364,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4367,17 +4378,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE11B0DB-5C62-420D-84D8-E87A9EF327B7}" name="表1" displayName="表1" ref="B1:J62" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" headerRowCellStyle="常规 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE11B0DB-5C62-420D-84D8-E87A9EF327B7}" name="表1" displayName="表1" ref="B1:J62" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" headerRowCellStyle="常规 2">
   <autoFilter ref="B1:J62" xr:uid="{B6969820-1EDF-4876-9A5D-FBFC4A41984D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{72E794A9-4DD1-49BE-A027-5ADCBA03FBD0}" name="列名/Column"/>
-    <tableColumn id="2" xr3:uid="{2BD92A17-8B86-4B03-9D18-9105A0D34354}" name="数据类型/Type" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{D8E94063-B8C9-4FA6-9A01-E7DF0C6D48F1}" name="长度/Length" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{9C5A6399-4D88-4569-8E5F-39B9DE8AF37B}" name="是否为空/Null(Y,N)" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{A4F55127-F997-4CC4-B0D1-1DA0A350A101}" name="默认值/Default" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{0F626792-F279-49AC-8EC1-BFB6B6687D67}" name="是否主键/Primary(Y,N)" dataDxfId="63"/>
-    <tableColumn id="7" xr3:uid="{7071273C-D0E4-4535-8AE8-1DA697EFE72A}" name="是否唯一/Unique(Y,N)" dataDxfId="62"/>
-    <tableColumn id="8" xr3:uid="{79AD77F4-4A81-4B14-B022-EB542F9CB50D}" name="外键/Forigen(可空)" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{2BD92A17-8B86-4B03-9D18-9105A0D34354}" name="数据类型/Type" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{D8E94063-B8C9-4FA6-9A01-E7DF0C6D48F1}" name="长度/Length" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{9C5A6399-4D88-4569-8E5F-39B9DE8AF37B}" name="是否为空/Null(Y,N)" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{A4F55127-F997-4CC4-B0D1-1DA0A350A101}" name="默认值/Default" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{0F626792-F279-49AC-8EC1-BFB6B6687D67}" name="是否主键/Primary(Y,N)" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{7071273C-D0E4-4535-8AE8-1DA697EFE72A}" name="是否唯一/Unique(Y,N)" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{79AD77F4-4A81-4B14-B022-EB542F9CB50D}" name="外键/Forigen(可空)" dataDxfId="66"/>
     <tableColumn id="9" xr3:uid="{F4869BE7-97E9-4573-A762-3FCC07598356}" name="备注/Comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4385,18 +4396,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D4223DF3-0FD4-4A51-9CB4-4ADBF0194284}" name="表4" displayName="表4" ref="B1:J124" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" headerRowCellStyle="常规 2">
-  <autoFilter ref="B1:J124" xr:uid="{B9CDCF83-4341-4D97-8AF8-098A114465A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D4223DF3-0FD4-4A51-9CB4-4ADBF0194284}" name="表4" displayName="表4" ref="B1:J125" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" headerRowCellStyle="常规 2">
+  <autoFilter ref="B1:J125" xr:uid="{B9CDCF83-4341-4D97-8AF8-098A114465A9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{350E8EA7-6A95-4955-AF92-86AAEA2BA677}" name="列名/Column" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{6ABB1A04-FB0D-4D10-B245-B8C8DB4828E1}" name="数据类型/Type" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{FCA6C0C7-D58A-4EB4-ADAD-587CBD0DD701}" name="长度/Length" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{52DA6CEC-27BC-4EAE-AE94-7470B76EC7C3}" name="是否为空/Null(Y,N)" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{AE35D0B9-0729-44FC-B690-C7EDD3166A02}" name="默认值/Default" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{6C52994F-377C-4C2E-9F7E-525CAC70A537}" name="是否主键/Primary(Y,N)" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{6EA4723E-17A5-4EC8-8998-8102D06DE919}" name="是否唯一/Unique(Y,N)" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{1A6BD3A8-4916-46D9-B4C6-624DA102515A}" name="外键/Forigen(可空)" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{632B0B2F-EABB-4492-9536-4E24187636CD}" name="备注/Comment" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{350E8EA7-6A95-4955-AF92-86AAEA2BA677}" name="列名/Column" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{6ABB1A04-FB0D-4D10-B245-B8C8DB4828E1}" name="数据类型/Type" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{FCA6C0C7-D58A-4EB4-ADAD-587CBD0DD701}" name="长度/Length" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{52DA6CEC-27BC-4EAE-AE94-7470B76EC7C3}" name="是否为空/Null(Y,N)" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{AE35D0B9-0729-44FC-B690-C7EDD3166A02}" name="默认值/Default" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{6C52994F-377C-4C2E-9F7E-525CAC70A537}" name="是否主键/Primary(Y,N)" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{6EA4723E-17A5-4EC8-8998-8102D06DE919}" name="是否唯一/Unique(Y,N)" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{1A6BD3A8-4916-46D9-B4C6-624DA102515A}" name="外键/Forigen(可空)" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{632B0B2F-EABB-4492-9536-4E24187636CD}" name="备注/Comment" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4662,8 +4673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4909,8 +4920,8 @@
       <c r="B11" t="s">
         <v>896</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>718</v>
+      <c r="C11" s="60" t="s">
+        <v>738</v>
       </c>
       <c r="D11" s="28"/>
       <c r="J11" t="s">
@@ -5110,8 +5121,8 @@
       <c r="B23" t="s">
         <v>896</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>718</v>
+      <c r="C23" s="60" t="s">
+        <v>900</v>
       </c>
       <c r="D23" s="28"/>
       <c r="J23" s="23" t="s">
@@ -5255,7 +5266,7 @@
         <v>899</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D32" s="28"/>
       <c r="J32" t="s">
@@ -5358,7 +5369,7 @@
         <v>896</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D39" s="28"/>
       <c r="J39" t="s">
@@ -5481,7 +5492,7 @@
         <v>896</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D47" s="28"/>
       <c r="J47" t="s">
@@ -5612,7 +5623,7 @@
         <v>899</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D56" s="28"/>
       <c r="J56" t="s">
@@ -5700,7 +5711,7 @@
         <v>899</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D62" s="28"/>
       <c r="J62" t="s">
@@ -5827,27 +5838,27 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="74" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:E1">
-    <cfRule type="cellIs" dxfId="73" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H1">
-    <cfRule type="cellIs" dxfId="72" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" dxfId="71" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="70" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5921,7 +5932,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>866</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -5945,7 +5956,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="29" t="s">
         <v>721</v>
       </c>
@@ -5965,7 +5976,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
+      <c r="A4" s="59"/>
       <c r="B4" s="29" t="s">
         <v>872</v>
       </c>
@@ -5985,7 +5996,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="29" t="s">
         <v>873</v>
       </c>
@@ -6005,7 +6016,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="29" t="s">
         <v>875</v>
       </c>
@@ -6025,7 +6036,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="29" t="s">
         <v>876</v>
       </c>
@@ -6045,7 +6056,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="29" t="s">
         <v>877</v>
       </c>
@@ -6065,7 +6076,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="29" t="s">
         <v>879</v>
       </c>
@@ -6085,7 +6096,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="29" t="s">
         <v>880</v>
       </c>
@@ -6105,7 +6116,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="37" t="s">
         <v>881</v>
       </c>
@@ -6125,7 +6136,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="29" t="s">
         <v>882</v>
       </c>
@@ -6145,7 +6156,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="29" t="s">
         <v>883</v>
       </c>
@@ -6165,7 +6176,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="29" t="s">
         <v>884</v>
       </c>
@@ -6183,7 +6194,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="29" t="s">
         <v>885</v>
       </c>
@@ -8397,10 +8408,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L132"/>
+  <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8450,7 +8461,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="57" t="s">
         <v>855</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -8472,7 +8483,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="29" t="s">
         <v>853</v>
       </c>
@@ -8492,7 +8503,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="33" t="s">
         <v>751</v>
       </c>
@@ -8512,7 +8523,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="29" t="s">
         <v>854</v>
       </c>
@@ -9047,7 +9058,7 @@
         <v>897</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>718</v>
+        <v>900</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="10"/>
@@ -9303,7 +9314,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="61" t="s">
         <v>726</v>
       </c>
       <c r="B40" s="21" t="s">
@@ -9325,7 +9336,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="58"/>
+      <c r="A41" s="5"/>
       <c r="B41" s="21" t="s">
         <v>125</v>
       </c>
@@ -9345,7 +9356,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="58"/>
+      <c r="A42" s="5"/>
       <c r="B42" s="21" t="s">
         <v>126</v>
       </c>
@@ -9365,7 +9376,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="58"/>
+      <c r="A43" s="5"/>
       <c r="B43" s="21" t="s">
         <v>127</v>
       </c>
@@ -9385,15 +9396,15 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
-      <c r="B44" s="21" t="s">
-        <v>128</v>
+      <c r="A44" s="5"/>
+      <c r="B44" s="29" t="s">
+        <v>901</v>
       </c>
       <c r="C44" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="30">
         <v>11</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>748</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -9401,19 +9412,19 @@
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
       <c r="J44" s="27" t="s">
-        <v>772</v>
+        <v>902</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="58"/>
+      <c r="A45" s="5"/>
       <c r="B45" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>20</v>
+        <v>748</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -9421,19 +9432,19 @@
       <c r="H45" s="24"/>
       <c r="I45" s="24"/>
       <c r="J45" s="27" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="58"/>
+      <c r="A46" s="5"/>
       <c r="B46" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
@@ -9441,19 +9452,19 @@
       <c r="H46" s="24"/>
       <c r="I46" s="24"/>
       <c r="J46" s="27" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="58"/>
+      <c r="A47" s="5"/>
       <c r="B47" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>748</v>
+        <v>12</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="24"/>
@@ -9461,19 +9472,19 @@
       <c r="H47" s="24"/>
       <c r="I47" s="24"/>
       <c r="J47" s="27" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="58"/>
+      <c r="A48" s="5"/>
       <c r="B48" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>12</v>
+        <v>748</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="24"/>
@@ -9481,19 +9492,19 @@
       <c r="H48" s="24"/>
       <c r="I48" s="24"/>
       <c r="J48" s="27" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="58"/>
+      <c r="A49" s="5"/>
       <c r="B49" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E49" s="24"/>
       <c r="F49" s="24"/>
@@ -9501,15 +9512,13 @@
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
       <c r="J49" s="27" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="55" t="s">
-        <v>728</v>
-      </c>
+      <c r="A50" s="5"/>
       <c r="B50" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>17</v>
@@ -9517,71 +9526,67 @@
       <c r="D50" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
       <c r="J50" s="27" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="55" t="s">
+        <v>728</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="27" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
-      <c r="B51" s="47" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="55"/>
+      <c r="B52" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C52" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D51" s="45" t="s">
+      <c r="D52" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="46" t="s">
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="23"/>
-      <c r="J52" s="27" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="56"/>
       <c r="B53" s="21" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>17</v>
@@ -9593,85 +9598,91 @@
         <v>13</v>
       </c>
       <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
+      <c r="G53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="I53" s="23"/>
       <c r="J53" s="27" t="s">
-        <v>771</v>
+        <v>779</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="55" t="s">
-        <v>841</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>840</v>
+      <c r="A54" s="56"/>
+      <c r="B54" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>748</v>
-      </c>
-      <c r="E54" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="23"/>
       <c r="J54" s="27" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="55" t="s">
+        <v>841</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>840</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="27" t="s">
         <v>780</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="47" t="s">
-        <v>836</v>
-      </c>
-      <c r="C55" s="44" t="s">
-        <v>709</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>748</v>
-      </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48"/>
-      <c r="J55" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="56"/>
-      <c r="B56" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="27" t="s">
-        <v>781</v>
+      <c r="B56" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C56" s="44" t="s">
+        <v>709</v>
+      </c>
+      <c r="D56" s="45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="46" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="56"/>
       <c r="B57" s="21" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>708</v>
+        <v>17</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
@@ -9679,21 +9690,19 @@
       <c r="H57" s="10"/>
       <c r="I57" s="23"/>
       <c r="J57" s="27" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="55" t="s">
-        <v>842</v>
-      </c>
+      <c r="A58" s="56"/>
       <c r="B58" s="21" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>11</v>
+        <v>708</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>748</v>
+        <v>24</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
@@ -9701,53 +9710,55 @@
       <c r="H58" s="10"/>
       <c r="I58" s="23"/>
       <c r="J58" s="27" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="55" t="s">
+        <v>842</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="27" t="s">
         <v>783</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="47" t="s">
-        <v>836</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>709</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>748</v>
-      </c>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="56"/>
-      <c r="B60" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="27" t="s">
-        <v>784</v>
+      <c r="B60" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C60" s="44" t="s">
+        <v>709</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="46" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="56"/>
       <c r="B61" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>17</v>
@@ -9761,19 +9772,19 @@
       <c r="H61" s="10"/>
       <c r="I61" s="23"/>
       <c r="J61" s="27" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="56"/>
       <c r="B62" s="21" t="s">
-        <v>856</v>
+        <v>142</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>730</v>
+        <v>35</v>
       </c>
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
@@ -9781,19 +9792,19 @@
       <c r="H62" s="10"/>
       <c r="I62" s="23"/>
       <c r="J62" s="27" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="56"/>
       <c r="B63" s="21" t="s">
-        <v>144</v>
+        <v>856</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>35</v>
+        <v>730</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
@@ -9801,16 +9812,16 @@
       <c r="H63" s="10"/>
       <c r="I63" s="23"/>
       <c r="J63" s="27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="56"/>
       <c r="B64" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>709</v>
+        <v>17</v>
       </c>
       <c r="D64" s="30" t="s">
         <v>35</v>
@@ -9821,16 +9832,16 @@
       <c r="H64" s="10"/>
       <c r="I64" s="23"/>
       <c r="J64" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="56"/>
       <c r="B65" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>17</v>
+        <v>709</v>
       </c>
       <c r="D65" s="30" t="s">
         <v>35</v>
@@ -9841,13 +9852,13 @@
       <c r="H65" s="10"/>
       <c r="I65" s="23"/>
       <c r="J65" s="27" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="56"/>
       <c r="B66" s="21" t="s">
-        <v>733</v>
+        <v>146</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>17</v>
@@ -9861,19 +9872,19 @@
       <c r="H66" s="10"/>
       <c r="I66" s="23"/>
       <c r="J66" s="27" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="56"/>
       <c r="B67" s="21" t="s">
-        <v>147</v>
+        <v>733</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
@@ -9881,19 +9892,19 @@
       <c r="H67" s="10"/>
       <c r="I67" s="23"/>
       <c r="J67" s="27" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="56"/>
       <c r="B68" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
@@ -9901,21 +9912,19 @@
       <c r="H68" s="10"/>
       <c r="I68" s="23"/>
       <c r="J68" s="27" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="55" t="s">
-        <v>843</v>
-      </c>
+      <c r="A69" s="56"/>
       <c r="B69" s="21" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>748</v>
+        <v>24</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
@@ -9923,53 +9932,55 @@
       <c r="H69" s="10"/>
       <c r="I69" s="23"/>
       <c r="J69" s="27" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="55" t="s">
+        <v>843</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="27" t="s">
         <v>780</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="56"/>
-      <c r="B70" s="47" t="s">
-        <v>836</v>
-      </c>
-      <c r="C70" s="44" t="s">
-        <v>709</v>
-      </c>
-      <c r="D70" s="45" t="s">
-        <v>748</v>
-      </c>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="56"/>
-      <c r="B71" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C71" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="27" t="s">
-        <v>793</v>
+      <c r="B71" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C71" s="44" t="s">
+        <v>709</v>
+      </c>
+      <c r="D71" s="45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="48"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="46" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="56"/>
       <c r="B72" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C72" s="22" t="s">
         <v>17</v>
@@ -9983,13 +9994,13 @@
       <c r="H72" s="24"/>
       <c r="I72" s="24"/>
       <c r="J72" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="56"/>
       <c r="B73" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C73" s="22" t="s">
         <v>17</v>
@@ -10003,19 +10014,19 @@
       <c r="H73" s="24"/>
       <c r="I73" s="24"/>
       <c r="J73" s="27" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="56"/>
       <c r="B74" s="21" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>707</v>
+        <v>35</v>
       </c>
       <c r="E74" s="24"/>
       <c r="F74" s="24"/>
@@ -10023,13 +10034,13 @@
       <c r="H74" s="24"/>
       <c r="I74" s="24"/>
       <c r="J74" s="27" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="56"/>
       <c r="B75" s="21" t="s">
-        <v>52</v>
+        <v>148</v>
       </c>
       <c r="C75" s="22" t="s">
         <v>23</v>
@@ -10043,19 +10054,19 @@
       <c r="H75" s="24"/>
       <c r="I75" s="24"/>
       <c r="J75" s="27" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="56"/>
       <c r="B76" s="21" t="s">
-        <v>742</v>
+        <v>52</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>27</v>
+        <v>707</v>
       </c>
       <c r="E76" s="24"/>
       <c r="F76" s="24"/>
@@ -10063,19 +10074,19 @@
       <c r="H76" s="24"/>
       <c r="I76" s="24"/>
       <c r="J76" s="27" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="56"/>
       <c r="B77" s="21" t="s">
-        <v>136</v>
+        <v>742</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>730</v>
+        <v>27</v>
       </c>
       <c r="E77" s="24"/>
       <c r="F77" s="24"/>
@@ -10083,55 +10094,55 @@
       <c r="H77" s="24"/>
       <c r="I77" s="24"/>
       <c r="J77" s="27" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="56"/>
+      <c r="B78" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>730</v>
+      </c>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="27" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="55" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="55" t="s">
         <v>844</v>
       </c>
-      <c r="B78" s="47" t="s">
+      <c r="B79" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C78" s="44" t="s">
+      <c r="C79" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D78" s="45" t="s">
+      <c r="D79" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E78" s="48"/>
-      <c r="F78" s="48"/>
-      <c r="G78" s="48"/>
-      <c r="H78" s="48"/>
-      <c r="I78" s="48"/>
-      <c r="J78" s="46" t="s">
+      <c r="E79" s="48"/>
+      <c r="F79" s="48"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="48"/>
+      <c r="I79" s="48"/>
+      <c r="J79" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="56"/>
-      <c r="B79" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="27" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="56"/>
       <c r="B80" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C80" s="22" t="s">
         <v>17</v>
@@ -10145,13 +10156,13 @@
       <c r="H80" s="24"/>
       <c r="I80" s="24"/>
       <c r="J80" s="27" t="s">
-        <v>798</v>
+        <v>731</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="56"/>
       <c r="B81" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C81" s="22" t="s">
         <v>17</v>
@@ -10165,13 +10176,13 @@
       <c r="H81" s="24"/>
       <c r="I81" s="24"/>
       <c r="J81" s="27" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="56"/>
       <c r="B82" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="22" t="s">
         <v>17</v>
@@ -10185,19 +10196,19 @@
       <c r="H82" s="24"/>
       <c r="I82" s="24"/>
       <c r="J82" s="27" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="56"/>
-      <c r="B83" s="29" t="s">
-        <v>856</v>
+      <c r="B83" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="C83" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>730</v>
+        <v>35</v>
       </c>
       <c r="E83" s="24"/>
       <c r="F83" s="24"/>
@@ -10205,19 +10216,19 @@
       <c r="H83" s="24"/>
       <c r="I83" s="24"/>
       <c r="J83" s="27" t="s">
-        <v>732</v>
+        <v>800</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="56"/>
-      <c r="B84" s="21" t="s">
-        <v>52</v>
+      <c r="B84" s="29" t="s">
+        <v>856</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>158</v>
+        <v>730</v>
       </c>
       <c r="E84" s="24"/>
       <c r="F84" s="24"/>
@@ -10225,21 +10236,19 @@
       <c r="H84" s="24"/>
       <c r="I84" s="24"/>
       <c r="J84" s="27" t="s">
-        <v>782</v>
+        <v>732</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="55" t="s">
-        <v>845</v>
-      </c>
+      <c r="A85" s="56"/>
       <c r="B85" s="21" t="s">
-        <v>159</v>
+        <v>52</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>748</v>
+        <v>158</v>
       </c>
       <c r="E85" s="24"/>
       <c r="F85" s="24"/>
@@ -10247,53 +10256,55 @@
       <c r="H85" s="24"/>
       <c r="I85" s="24"/>
       <c r="J85" s="27" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="55" t="s">
+        <v>845</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="27" t="s">
         <v>801</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="56"/>
-      <c r="B86" s="47" t="s">
-        <v>836</v>
-      </c>
-      <c r="C86" s="44" t="s">
-        <v>709</v>
-      </c>
-      <c r="D86" s="45" t="s">
-        <v>748</v>
-      </c>
-      <c r="E86" s="48"/>
-      <c r="F86" s="48"/>
-      <c r="G86" s="48"/>
-      <c r="H86" s="48"/>
-      <c r="I86" s="48"/>
-      <c r="J86" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="56"/>
-      <c r="B87" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
-      <c r="I87" s="24"/>
-      <c r="J87" s="27" t="s">
-        <v>802</v>
+      <c r="B87" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C87" s="44" t="s">
+        <v>709</v>
+      </c>
+      <c r="D87" s="45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E87" s="48"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
+      <c r="I87" s="48"/>
+      <c r="J87" s="46" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="56"/>
       <c r="B88" s="21" t="s">
-        <v>734</v>
+        <v>160</v>
       </c>
       <c r="C88" s="22" t="s">
         <v>17</v>
@@ -10307,13 +10318,13 @@
       <c r="H88" s="24"/>
       <c r="I88" s="24"/>
       <c r="J88" s="27" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="56"/>
       <c r="B89" s="21" t="s">
-        <v>161</v>
+        <v>734</v>
       </c>
       <c r="C89" s="22" t="s">
         <v>17</v>
@@ -10327,19 +10338,19 @@
       <c r="H89" s="24"/>
       <c r="I89" s="24"/>
       <c r="J89" s="27" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="56"/>
       <c r="B90" s="21" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E90" s="24"/>
       <c r="F90" s="24"/>
@@ -10347,21 +10358,19 @@
       <c r="H90" s="24"/>
       <c r="I90" s="24"/>
       <c r="J90" s="27" t="s">
-        <v>782</v>
+        <v>804</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="55" t="s">
-        <v>846</v>
-      </c>
+      <c r="A91" s="56"/>
       <c r="B91" s="21" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D91" s="30" t="s">
-        <v>748</v>
+        <v>24</v>
       </c>
       <c r="E91" s="24"/>
       <c r="F91" s="24"/>
@@ -10369,53 +10378,55 @@
       <c r="H91" s="24"/>
       <c r="I91" s="24"/>
       <c r="J91" s="27" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="55" t="s">
+        <v>846</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>748</v>
+      </c>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="27" t="s">
         <v>801</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="56"/>
-      <c r="B92" s="47" t="s">
-        <v>836</v>
-      </c>
-      <c r="C92" s="44" t="s">
-        <v>709</v>
-      </c>
-      <c r="D92" s="45" t="s">
-        <v>748</v>
-      </c>
-      <c r="E92" s="48"/>
-      <c r="F92" s="48"/>
-      <c r="G92" s="48"/>
-      <c r="H92" s="48"/>
-      <c r="I92" s="48"/>
-      <c r="J92" s="46" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="56"/>
-      <c r="B93" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
-      <c r="I93" s="24"/>
-      <c r="J93" s="27" t="s">
-        <v>805</v>
+      <c r="B93" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C93" s="44" t="s">
+        <v>709</v>
+      </c>
+      <c r="D93" s="45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E93" s="48"/>
+      <c r="F93" s="48"/>
+      <c r="G93" s="48"/>
+      <c r="H93" s="48"/>
+      <c r="I93" s="48"/>
+      <c r="J93" s="46" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="56"/>
       <c r="B94" s="21" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="C94" s="22" t="s">
         <v>17</v>
@@ -10429,13 +10440,13 @@
       <c r="H94" s="24"/>
       <c r="I94" s="24"/>
       <c r="J94" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="56"/>
       <c r="B95" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C95" s="22" t="s">
         <v>17</v>
@@ -10449,19 +10460,19 @@
       <c r="H95" s="24"/>
       <c r="I95" s="24"/>
       <c r="J95" s="27" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="56"/>
       <c r="B96" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C96" s="22" t="s">
-        <v>736</v>
+        <v>17</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>737</v>
+        <v>20</v>
       </c>
       <c r="E96" s="24"/>
       <c r="F96" s="24"/>
@@ -10469,55 +10480,55 @@
       <c r="H96" s="24"/>
       <c r="I96" s="24"/>
       <c r="J96" s="27" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="56"/>
+      <c r="B97" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>736</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>737</v>
+      </c>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24"/>
+      <c r="J97" s="27" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="55" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="55" t="s">
         <v>847</v>
       </c>
-      <c r="B97" s="47" t="s">
+      <c r="B98" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C97" s="44" t="s">
+      <c r="C98" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D97" s="45" t="s">
+      <c r="D98" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E97" s="48"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="48"/>
-      <c r="H97" s="48"/>
-      <c r="I97" s="48"/>
-      <c r="J97" s="46" t="s">
+      <c r="E98" s="48"/>
+      <c r="F98" s="48"/>
+      <c r="G98" s="48"/>
+      <c r="H98" s="48"/>
+      <c r="I98" s="48"/>
+      <c r="J98" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="56"/>
-      <c r="B98" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>729</v>
-      </c>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="24"/>
-      <c r="I98" s="24"/>
-      <c r="J98" s="27" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="56"/>
       <c r="B99" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C99" s="22" t="s">
         <v>11</v>
@@ -10531,55 +10542,55 @@
       <c r="H99" s="24"/>
       <c r="I99" s="24"/>
       <c r="J99" s="27" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="56"/>
+      <c r="B100" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>729</v>
+      </c>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24"/>
+      <c r="J100" s="27" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="55" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="55" t="s">
         <v>848</v>
       </c>
-      <c r="B100" s="47" t="s">
+      <c r="B101" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C100" s="44" t="s">
+      <c r="C101" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D100" s="45" t="s">
+      <c r="D101" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E100" s="48"/>
-      <c r="F100" s="48"/>
-      <c r="G100" s="48"/>
-      <c r="H100" s="48"/>
-      <c r="I100" s="48"/>
-      <c r="J100" s="46" t="s">
+      <c r="E101" s="48"/>
+      <c r="F101" s="48"/>
+      <c r="G101" s="48"/>
+      <c r="H101" s="48"/>
+      <c r="I101" s="48"/>
+      <c r="J101" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="56"/>
-      <c r="B101" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C101" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="30" t="s">
-        <v>729</v>
-      </c>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
-      <c r="I101" s="24"/>
-      <c r="J101" s="27" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="56"/>
       <c r="B102" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C102" s="22" t="s">
         <v>11</v>
@@ -10593,55 +10604,55 @@
       <c r="H102" s="24"/>
       <c r="I102" s="24"/>
       <c r="J102" s="27" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="56"/>
+      <c r="B103" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>729</v>
+      </c>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="27" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="55" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="55" t="s">
         <v>849</v>
       </c>
-      <c r="B103" s="47" t="s">
+      <c r="B104" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C103" s="44" t="s">
+      <c r="C104" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D103" s="45" t="s">
+      <c r="D104" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E103" s="48"/>
-      <c r="F103" s="48"/>
-      <c r="G103" s="48"/>
-      <c r="H103" s="48"/>
-      <c r="I103" s="48"/>
-      <c r="J103" s="46" t="s">
+      <c r="E104" s="48"/>
+      <c r="F104" s="48"/>
+      <c r="G104" s="48"/>
+      <c r="H104" s="48"/>
+      <c r="I104" s="48"/>
+      <c r="J104" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="56"/>
-      <c r="B104" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>729</v>
-      </c>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
-      <c r="I104" s="24"/>
-      <c r="J104" s="27" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="56"/>
       <c r="B105" s="21" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C105" s="22" t="s">
         <v>11</v>
@@ -10655,55 +10666,55 @@
       <c r="H105" s="24"/>
       <c r="I105" s="24"/>
       <c r="J105" s="27" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="56"/>
+      <c r="B106" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>729</v>
+      </c>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+      <c r="I106" s="24"/>
+      <c r="J106" s="27" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="55" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="55" t="s">
         <v>850</v>
       </c>
-      <c r="B106" s="47" t="s">
+      <c r="B107" s="47" t="s">
         <v>836</v>
       </c>
-      <c r="C106" s="44" t="s">
+      <c r="C107" s="44" t="s">
         <v>709</v>
       </c>
-      <c r="D106" s="45" t="s">
+      <c r="D107" s="45" t="s">
         <v>748</v>
       </c>
-      <c r="E106" s="48"/>
-      <c r="F106" s="48"/>
-      <c r="G106" s="48"/>
-      <c r="H106" s="48"/>
-      <c r="I106" s="48"/>
-      <c r="J106" s="46" t="s">
+      <c r="E107" s="48"/>
+      <c r="F107" s="48"/>
+      <c r="G107" s="48"/>
+      <c r="H107" s="48"/>
+      <c r="I107" s="48"/>
+      <c r="J107" s="46" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="56"/>
-      <c r="B107" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="30" t="s">
-        <v>729</v>
-      </c>
-      <c r="E107" s="24"/>
-      <c r="F107" s="24"/>
-      <c r="G107" s="24"/>
-      <c r="H107" s="24"/>
-      <c r="I107" s="24"/>
-      <c r="J107" s="27" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="56"/>
       <c r="B108" s="21" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C108" s="22" t="s">
         <v>11</v>
@@ -10717,21 +10728,19 @@
       <c r="H108" s="24"/>
       <c r="I108" s="24"/>
       <c r="J108" s="27" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="59" t="s">
-        <v>172</v>
-      </c>
+      <c r="A109" s="56"/>
       <c r="B109" s="21" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="C109" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D109" s="30">
-        <v>19</v>
+      <c r="D109" s="30" t="s">
+        <v>729</v>
       </c>
       <c r="E109" s="24"/>
       <c r="F109" s="24"/>
@@ -10739,19 +10748,21 @@
       <c r="H109" s="24"/>
       <c r="I109" s="24"/>
       <c r="J109" s="27" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="59"/>
-      <c r="B110" s="29" t="s">
-        <v>857</v>
+      <c r="A110" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>706</v>
+        <v>11</v>
+      </c>
+      <c r="D110" s="30">
+        <v>19</v>
       </c>
       <c r="E110" s="24"/>
       <c r="F110" s="24"/>
@@ -10759,19 +10770,19 @@
       <c r="H110" s="24"/>
       <c r="I110" s="24"/>
       <c r="J110" s="27" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="59"/>
-      <c r="B111" s="21" t="s">
-        <v>174</v>
+      <c r="A111" s="54"/>
+      <c r="B111" s="29" t="s">
+        <v>857</v>
       </c>
       <c r="C111" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D111" s="30">
-        <v>32</v>
+      <c r="D111" s="30" t="s">
+        <v>706</v>
       </c>
       <c r="E111" s="24"/>
       <c r="F111" s="24"/>
@@ -10779,19 +10790,19 @@
       <c r="H111" s="24"/>
       <c r="I111" s="24"/>
       <c r="J111" s="27" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="59"/>
+      <c r="A112" s="54"/>
       <c r="B112" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C112" s="22" t="s">
-        <v>708</v>
+        <v>17</v>
       </c>
       <c r="D112" s="30">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E112" s="24"/>
       <c r="F112" s="24"/>
@@ -10799,21 +10810,19 @@
       <c r="H112" s="24"/>
       <c r="I112" s="24"/>
       <c r="J112" s="27" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="59" t="s">
-        <v>176</v>
-      </c>
+      <c r="A113" s="54"/>
       <c r="B113" s="21" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="C113" s="22" t="s">
-        <v>11</v>
+        <v>708</v>
       </c>
       <c r="D113" s="30">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E113" s="24"/>
       <c r="F113" s="24"/>
@@ -10821,19 +10830,21 @@
       <c r="H113" s="24"/>
       <c r="I113" s="24"/>
       <c r="J113" s="27" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="59"/>
+      <c r="A114" s="54" t="s">
+        <v>176</v>
+      </c>
       <c r="B114" s="21" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="C114" s="22" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D114" s="30">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E114" s="24"/>
       <c r="F114" s="24"/>
@@ -10841,19 +10852,19 @@
       <c r="H114" s="24"/>
       <c r="I114" s="24"/>
       <c r="J114" s="27" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="59"/>
+      <c r="A115" s="54"/>
       <c r="B115" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C115" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D115" s="30">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E115" s="24"/>
       <c r="F115" s="24"/>
@@ -10861,19 +10872,19 @@
       <c r="H115" s="24"/>
       <c r="I115" s="24"/>
       <c r="J115" s="27" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="59"/>
+      <c r="A116" s="54"/>
       <c r="B116" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C116" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D116" s="30">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E116" s="24"/>
       <c r="F116" s="24"/>
@@ -10881,21 +10892,19 @@
       <c r="H116" s="24"/>
       <c r="I116" s="24"/>
       <c r="J116" s="27" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="59" t="s">
-        <v>180</v>
-      </c>
+      <c r="A117" s="54"/>
       <c r="B117" s="21" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="C117" s="22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D117" s="30">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E117" s="24"/>
       <c r="F117" s="24"/>
@@ -10903,19 +10912,21 @@
       <c r="H117" s="24"/>
       <c r="I117" s="24"/>
       <c r="J117" s="27" t="s">
-        <v>814</v>
+        <v>820</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="59"/>
+      <c r="A118" s="54" t="s">
+        <v>180</v>
+      </c>
       <c r="B118" s="21" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="C118" s="22" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D118" s="30">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E118" s="24"/>
       <c r="F118" s="24"/>
@@ -10923,31 +10934,33 @@
       <c r="H118" s="24"/>
       <c r="I118" s="24"/>
       <c r="J118" s="27" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="59"/>
+      <c r="A119" s="54"/>
       <c r="B119" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C119" s="22" t="s">
-        <v>738</v>
-      </c>
-      <c r="D119" s="30"/>
+        <v>23</v>
+      </c>
+      <c r="D119" s="30">
+        <v>3</v>
+      </c>
       <c r="E119" s="24"/>
       <c r="F119" s="24"/>
       <c r="G119" s="24"/>
       <c r="H119" s="24"/>
       <c r="I119" s="24"/>
       <c r="J119" s="27" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="59"/>
+      <c r="A120" s="54"/>
       <c r="B120" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C120" s="22" t="s">
         <v>738</v>
@@ -10959,41 +10972,39 @@
       <c r="H120" s="24"/>
       <c r="I120" s="24"/>
       <c r="J120" s="27" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="59" t="s">
-        <v>835</v>
-      </c>
+      <c r="A121" s="54"/>
       <c r="B121" s="21" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="C121" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D121" s="30">
-        <v>19</v>
-      </c>
+        <v>738</v>
+      </c>
+      <c r="D121" s="30"/>
       <c r="E121" s="24"/>
       <c r="F121" s="24"/>
       <c r="G121" s="24"/>
       <c r="H121" s="24"/>
       <c r="I121" s="24"/>
       <c r="J121" s="27" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="59"/>
-      <c r="B122" s="29" t="s">
-        <v>858</v>
+      <c r="A122" s="54" t="s">
+        <v>835</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="C122" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D122" s="30" t="s">
-        <v>706</v>
+        <v>11</v>
+      </c>
+      <c r="D122" s="30">
+        <v>19</v>
       </c>
       <c r="E122" s="24"/>
       <c r="F122" s="24"/>
@@ -11001,52 +11012,69 @@
       <c r="H122" s="24"/>
       <c r="I122" s="24"/>
       <c r="J122" s="27" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="59"/>
-      <c r="B123" s="21" t="s">
-        <v>184</v>
+      <c r="A123" s="54"/>
+      <c r="B123" s="29" t="s">
+        <v>858</v>
       </c>
       <c r="C123" s="22" t="s">
-        <v>738</v>
-      </c>
-      <c r="D123" s="30"/>
+        <v>17</v>
+      </c>
+      <c r="D123" s="30" t="s">
+        <v>706</v>
+      </c>
       <c r="E123" s="24"/>
       <c r="F123" s="24"/>
       <c r="G123" s="24"/>
       <c r="H123" s="24"/>
       <c r="I123" s="24"/>
       <c r="J123" s="27" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="59"/>
+      <c r="A124" s="54"/>
       <c r="B124" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C124" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D124" s="30">
-        <v>512</v>
-      </c>
+        <v>738</v>
+      </c>
+      <c r="D124" s="30"/>
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
       <c r="G124" s="24"/>
       <c r="H124" s="24"/>
       <c r="I124" s="24"/>
       <c r="J124" s="27" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="54"/>
+      <c r="B125" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C125" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D125" s="30">
+        <v>512</v>
+      </c>
+      <c r="E125" s="24"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="24"/>
+      <c r="J125" s="27" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="21"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C127" s="26"/>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" s="21"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C128" s="26"/>
@@ -11059,57 +11087,59 @@
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131" s="26"/>
-      <c r="D131" s="22"/>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C132" s="26"/>
       <c r="D132" s="22"/>
     </row>
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A109:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A68"/>
-    <mergeCell ref="A78:A84"/>
+  <mergeCells count="19">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A29"/>
-    <mergeCell ref="A69:A77"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A70:A78"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A92:A97"/>
     <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A51:A54"/>
     <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A69"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="A122:A125"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="A114:A117"/>
+    <mergeCell ref="A107:A109"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="60" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:E1">
-    <cfRule type="cellIs" dxfId="59" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:H1">
-    <cfRule type="cellIs" dxfId="58" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" dxfId="57" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11176,7 +11206,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>186</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -11204,7 +11234,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="15" t="s">
         <v>136</v>
       </c>
@@ -11230,7 +11260,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A4" s="60"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="15" t="s">
         <v>137</v>
       </c>
@@ -11256,7 +11286,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="15" t="s">
         <v>190</v>
       </c>
@@ -11282,7 +11312,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A6" s="60"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="15" t="s">
         <v>192</v>
       </c>
@@ -11308,7 +11338,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A7" s="60"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="15" t="s">
         <v>194</v>
       </c>
@@ -11334,7 +11364,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="15" t="s">
         <v>196</v>
       </c>
@@ -11360,7 +11390,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="15" t="s">
         <v>198</v>
       </c>
@@ -11386,7 +11416,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="15" t="s">
         <v>148</v>
       </c>
@@ -11412,7 +11442,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="15" t="s">
         <v>201</v>
       </c>
@@ -11438,7 +11468,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="12" t="s">
         <v>203</v>
       </c>
@@ -11464,7 +11494,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="12" t="s">
         <v>205</v>
       </c>
@@ -11490,7 +11520,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="15" t="s">
         <v>207</v>
       </c>
@@ -11516,7 +11546,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="58" t="s">
         <v>209</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -11544,7 +11574,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="12" t="s">
         <v>212</v>
       </c>
@@ -11570,7 +11600,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A17" s="60"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="12" t="s">
         <v>214</v>
       </c>
@@ -11596,7 +11626,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A18" s="60"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="12" t="s">
         <v>216</v>
       </c>
@@ -11622,7 +11652,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="12" t="s">
         <v>218</v>
       </c>
@@ -11648,7 +11678,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="12" t="s">
         <v>220</v>
       </c>
@@ -11674,7 +11704,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="12" t="s">
         <v>222</v>
       </c>
@@ -11700,7 +11730,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A22" s="60"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="12" t="s">
         <v>224</v>
       </c>
@@ -11726,7 +11756,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A23" s="60"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="12" t="s">
         <v>226</v>
       </c>
@@ -11752,7 +11782,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A24" s="60"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="12" t="s">
         <v>228</v>
       </c>
@@ -11778,7 +11808,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A25" s="60"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="12" t="s">
         <v>52</v>
       </c>
@@ -11804,7 +11834,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="58" t="s">
         <v>230</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -11832,7 +11862,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A27" s="60"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="15" t="s">
         <v>233</v>
       </c>
@@ -11858,7 +11888,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A28" s="60"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="15" t="s">
         <v>234</v>
       </c>
@@ -11884,7 +11914,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A29" s="60"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="15" t="s">
         <v>52</v>
       </c>
@@ -11910,7 +11940,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="58" t="s">
         <v>236</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -11938,7 +11968,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A31" s="60"/>
+      <c r="A31" s="58"/>
       <c r="B31" s="15" t="s">
         <v>201</v>
       </c>
@@ -11964,7 +11994,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A32" s="60"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="15" t="s">
         <v>240</v>
       </c>
@@ -11990,7 +12020,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A33" s="60"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="15" t="s">
         <v>52</v>
       </c>
@@ -12016,7 +12046,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="58" t="s">
         <v>242</v>
       </c>
       <c r="B34" s="15" t="s">
@@ -12044,7 +12074,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A35" s="60"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="15" t="s">
         <v>245</v>
       </c>
@@ -12070,7 +12100,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A36" s="60"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="15" t="s">
         <v>247</v>
       </c>
@@ -12096,7 +12126,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A37" s="60"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="15" t="s">
         <v>52</v>
       </c>
@@ -12122,7 +12152,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A38" s="60" t="s">
+      <c r="A38" s="58" t="s">
         <v>249</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -12150,7 +12180,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A39" s="60"/>
+      <c r="A39" s="58"/>
       <c r="B39" s="15" t="s">
         <v>250</v>
       </c>
@@ -12176,7 +12206,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A40" s="60"/>
+      <c r="A40" s="58"/>
       <c r="B40" s="15" t="s">
         <v>252</v>
       </c>
@@ -12202,7 +12232,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A41" s="60"/>
+      <c r="A41" s="58"/>
       <c r="B41" s="15" t="s">
         <v>201</v>
       </c>
@@ -12228,7 +12258,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="58" t="s">
         <v>254</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -12256,7 +12286,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
+      <c r="A43" s="58"/>
       <c r="B43" s="12" t="s">
         <v>255</v>
       </c>
@@ -12282,7 +12312,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A44" s="60"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="12" t="s">
         <v>257</v>
       </c>
@@ -12308,7 +12338,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="12" t="s">
         <v>259</v>
       </c>
@@ -12334,7 +12364,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A46" s="60"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="12" t="s">
         <v>261</v>
       </c>
@@ -12360,7 +12390,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A47" s="60"/>
+      <c r="A47" s="58"/>
       <c r="B47" s="12" t="s">
         <v>263</v>
       </c>
@@ -12386,7 +12416,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A48" s="60"/>
+      <c r="A48" s="58"/>
       <c r="B48" s="12" t="s">
         <v>265</v>
       </c>
@@ -12412,7 +12442,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A49" s="60"/>
+      <c r="A49" s="58"/>
       <c r="B49" s="12" t="s">
         <v>267</v>
       </c>
@@ -12438,7 +12468,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A50" s="60"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="12" t="s">
         <v>269</v>
       </c>
@@ -12464,7 +12494,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A51" s="60"/>
+      <c r="A51" s="58"/>
       <c r="B51" s="12" t="s">
         <v>271</v>
       </c>
@@ -12490,7 +12520,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="58" t="s">
         <v>273</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -12518,7 +12548,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A53" s="60"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="12" t="s">
         <v>275</v>
       </c>
@@ -12544,7 +12574,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A54" s="60"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="12" t="s">
         <v>277</v>
       </c>
@@ -12570,7 +12600,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A55" s="60"/>
+      <c r="A55" s="58"/>
       <c r="B55" s="12" t="s">
         <v>279</v>
       </c>
@@ -12596,7 +12626,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
+      <c r="A56" s="58"/>
       <c r="B56" s="12" t="s">
         <v>281</v>
       </c>
@@ -12622,7 +12652,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A57" s="60"/>
+      <c r="A57" s="58"/>
       <c r="B57" s="12" t="s">
         <v>282</v>
       </c>
@@ -12648,7 +12678,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A58" s="60"/>
+      <c r="A58" s="58"/>
       <c r="B58" s="12" t="s">
         <v>19</v>
       </c>
@@ -12674,7 +12704,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A59" s="60"/>
+      <c r="A59" s="58"/>
       <c r="B59" s="12" t="s">
         <v>261</v>
       </c>
@@ -12700,7 +12730,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A60" s="60"/>
+      <c r="A60" s="58"/>
       <c r="B60" s="12" t="s">
         <v>284</v>
       </c>
@@ -12726,7 +12756,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A61" s="60"/>
+      <c r="A61" s="58"/>
       <c r="B61" s="12" t="s">
         <v>263</v>
       </c>
@@ -12752,7 +12782,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A62" s="60"/>
+      <c r="A62" s="58"/>
       <c r="B62" s="12" t="s">
         <v>257</v>
       </c>
@@ -12778,7 +12808,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A63" s="60"/>
+      <c r="A63" s="58"/>
       <c r="B63" s="12" t="s">
         <v>286</v>
       </c>
@@ -12804,7 +12834,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A64" s="60"/>
+      <c r="A64" s="58"/>
       <c r="B64" s="12" t="s">
         <v>265</v>
       </c>
@@ -12830,7 +12860,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A65" s="60"/>
+      <c r="A65" s="58"/>
       <c r="B65" s="12" t="s">
         <v>288</v>
       </c>
@@ -12856,7 +12886,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A66" s="60"/>
+      <c r="A66" s="58"/>
       <c r="B66" s="12" t="s">
         <v>289</v>
       </c>
@@ -12882,7 +12912,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A67" s="60"/>
+      <c r="A67" s="58"/>
       <c r="B67" s="12" t="s">
         <v>267</v>
       </c>
@@ -12908,7 +12938,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A68" s="60"/>
+      <c r="A68" s="58"/>
       <c r="B68" s="12" t="s">
         <v>290</v>
       </c>
@@ -12934,7 +12964,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A69" s="60"/>
+      <c r="A69" s="58"/>
       <c r="B69" s="12" t="s">
         <v>201</v>
       </c>
@@ -12960,7 +12990,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A70" s="60"/>
+      <c r="A70" s="58"/>
       <c r="B70" s="12" t="s">
         <v>293</v>
       </c>
@@ -12986,7 +13016,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A71" s="60"/>
+      <c r="A71" s="58"/>
       <c r="B71" s="12" t="s">
         <v>294</v>
       </c>
@@ -13012,7 +13042,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A72" s="60"/>
+      <c r="A72" s="58"/>
       <c r="B72" s="12" t="s">
         <v>295</v>
       </c>
@@ -13038,7 +13068,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A73" s="60"/>
+      <c r="A73" s="58"/>
       <c r="B73" s="12" t="s">
         <v>296</v>
       </c>
@@ -13064,7 +13094,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A74" s="60"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="12" t="s">
         <v>198</v>
       </c>
@@ -13090,7 +13120,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A75" s="60"/>
+      <c r="A75" s="58"/>
       <c r="B75" s="12" t="s">
         <v>297</v>
       </c>
@@ -13116,7 +13146,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A76" s="60"/>
+      <c r="A76" s="58"/>
       <c r="B76" s="12" t="s">
         <v>299</v>
       </c>
@@ -13142,7 +13172,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A77" s="60"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="12" t="s">
         <v>300</v>
       </c>
@@ -13168,7 +13198,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A78" s="60"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="12" t="s">
         <v>301</v>
       </c>
@@ -13194,7 +13224,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A79" s="60"/>
+      <c r="A79" s="58"/>
       <c r="B79" s="12" t="s">
         <v>302</v>
       </c>
@@ -13220,7 +13250,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A80" s="60"/>
+      <c r="A80" s="58"/>
       <c r="B80" s="12" t="s">
         <v>303</v>
       </c>
@@ -13246,7 +13276,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A81" s="60"/>
+      <c r="A81" s="58"/>
       <c r="B81" s="12" t="s">
         <v>304</v>
       </c>
@@ -13272,7 +13302,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A82" s="60"/>
+      <c r="A82" s="58"/>
       <c r="B82" s="12" t="s">
         <v>305</v>
       </c>
@@ -13298,7 +13328,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A83" s="60"/>
+      <c r="A83" s="58"/>
       <c r="B83" s="12" t="s">
         <v>306</v>
       </c>
@@ -13324,7 +13354,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A84" s="60"/>
+      <c r="A84" s="58"/>
       <c r="B84" s="12" t="s">
         <v>307</v>
       </c>
@@ -13350,7 +13380,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A85" s="60"/>
+      <c r="A85" s="58"/>
       <c r="B85" s="12" t="s">
         <v>259</v>
       </c>
@@ -13376,7 +13406,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A86" s="60"/>
+      <c r="A86" s="58"/>
       <c r="B86" s="12" t="s">
         <v>308</v>
       </c>
@@ -13402,7 +13432,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A87" s="60"/>
+      <c r="A87" s="58"/>
       <c r="B87" s="12" t="s">
         <v>309</v>
       </c>
@@ -13428,7 +13458,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A88" s="60"/>
+      <c r="A88" s="58"/>
       <c r="B88" s="12" t="s">
         <v>311</v>
       </c>
@@ -13454,7 +13484,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A89" s="60"/>
+      <c r="A89" s="58"/>
       <c r="B89" s="12" t="s">
         <v>313</v>
       </c>
@@ -13480,7 +13510,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A90" s="60"/>
+      <c r="A90" s="58"/>
       <c r="B90" s="12" t="s">
         <v>315</v>
       </c>
@@ -13506,7 +13536,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A91" s="60"/>
+      <c r="A91" s="58"/>
       <c r="B91" s="12" t="s">
         <v>317</v>
       </c>
@@ -13532,7 +13562,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A92" s="60"/>
+      <c r="A92" s="58"/>
       <c r="B92" s="12" t="s">
         <v>318</v>
       </c>
@@ -13558,7 +13588,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A93" s="60" t="s">
+      <c r="A93" s="58" t="s">
         <v>320</v>
       </c>
       <c r="B93" s="12" t="s">
@@ -13586,7 +13616,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A94" s="60"/>
+      <c r="A94" s="58"/>
       <c r="B94" s="12" t="s">
         <v>322</v>
       </c>

</xml_diff>